<commit_message>
Separating functionality into general objects
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -12,11 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>This is a string</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51,8 +47,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -67,16 +64,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1.0</v>
+        <v>42894.35944359954</v>
       </c>
-      <c r="B1" t="n">
-        <v>1.2</v>
+      <c r="B1" t="n" s="1">
+        <v>42894.35944395833</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="b">
-        <v>1</v>
+      <c r="C1" t="n" s="1">
+        <v>42894.35944395833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added another cell manipulation function.
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -12,7 +12,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>a string</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,9 +51,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -62,15 +65,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>42894.35944359954</v>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.1</v>
       </c>
-      <c r="B1" t="n" s="1">
-        <v>42894.35944395833</v>
+      <c r="B3" t="n">
+        <v>42894.36889262732</v>
       </c>
-      <c r="C1" t="n" s="1">
-        <v>42894.35944395833</v>
+      <c r="C3" t="n">
+        <v>42894.36889262732</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added CellAlignment Scala Object.  This demos how to change cell alignments.
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="new sheet" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet0" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>a string</t>
+    <t>Align It</t>
   </si>
 </sst>
 </file>
@@ -51,8 +51,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -65,21 +68,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>42894.36889262732</v>
-      </c>
-      <c r="C3" t="n">
-        <v>42894.36889262732</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="3" ht="50.0" customHeight="true">
+      <c r="D3" t="s" s="1">
         <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>